<commit_message>
sistem yang berjalan dan perencanaan
</commit_message>
<xml_diff>
--- a/Design Database Application.xlsx
+++ b/Design Database Application.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hilda\Documents\Azwar\MySkripsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDAEF31-5714-4B2D-95AF-4C1F18E95523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09E4855-BFDC-4A24-83C6-2059F3D8BE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="99">
   <si>
     <t>Field</t>
   </si>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t>na</t>
+  </si>
+  <si>
+    <t>tb_pendidikan_user</t>
   </si>
 </sst>
 </file>
@@ -385,10 +388,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:AG33"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE8" sqref="AE8:AG9"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -715,46 +718,46 @@
       <c r="E5" s="1"/>
     </row>
     <row r="8" spans="1:33" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="G8" s="4" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="G8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="K8" s="4" t="s">
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="K8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="O8" s="4" t="s">
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="O8" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="S8" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-      <c r="W8" s="4" t="s">
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="S8" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="W8" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-      <c r="AA8" s="4" t="s">
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="AA8" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AB8" s="4"/>
-      <c r="AC8" s="4"/>
-      <c r="AE8" s="4" t="s">
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="5"/>
+      <c r="AE8" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AF8" s="4"/>
-      <c r="AG8" s="4"/>
+      <c r="AF8" s="5"/>
+      <c r="AG8" s="5"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="C9" s="3" t="s">
@@ -1059,7 +1062,7 @@
       <c r="H13" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="4" t="s">
         <v>70</v>
       </c>
       <c r="K13" t="s">
@@ -1552,7 +1555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72807FE2-8500-4B14-AA72-4BA4DA95C1CB}">
   <dimension ref="C4:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -1565,16 +1568,16 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="G4" s="4" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="G4" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C5" s="3" t="s">

</xml_diff>

<commit_message>
add draf hasil 2
</commit_message>
<xml_diff>
--- a/Design Database Application.xlsx
+++ b/Design Database Application.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hilda\Documents\Azwar\MySkripsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09E4855-BFDC-4A24-83C6-2059F3D8BE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42E2B88-D638-41FE-A020-FF96F7565AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="102">
   <si>
     <t>Field</t>
   </si>
@@ -323,6 +323,15 @@
   </si>
   <si>
     <t>tb_pendidikan_user</t>
+  </si>
+  <si>
+    <t>whatsapp</t>
+  </si>
+  <si>
+    <t>izinkan whatsapp</t>
+  </si>
+  <si>
+    <t>boolean</t>
   </si>
 </sst>
 </file>
@@ -672,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:AG33"/>
+  <dimension ref="A3:AG36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1533,6 +1542,19 @@
       </c>
       <c r="E33" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>